<commit_message>
Minor changes in document information.
</commit_message>
<xml_diff>
--- a/Documents/July/Acta_N°5.xlsx
+++ b/Documents/July/Acta_N°5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f23d3a1470f2609/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f23d3a1470f2609/Escritorio/Stationery/Documents/July/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08CE6100-11C7-496A-BB27-F5F9AAB1DDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{08CE6100-11C7-496A-BB27-F5F9AAB1DDE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BD2F7F7-5C82-4CA6-9B9D-97DDBB0FDBE5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,13 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>L. Baz
-F. Behn
-F. Jordán
-N. Núñez</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Acta de reunión</t>
   </si>
@@ -113,6 +107,14 @@
       </rPr>
       <t xml:space="preserve"> para hacer estos cambios y podremos corregir lo que ya está hecho?</t>
     </r>
+  </si>
+  <si>
+    <t>Actualizar a N. Núñez con las tareas pendientes.</t>
+  </si>
+  <si>
+    <t>L. Baz
+F. Behn
+F. Jordán</t>
   </si>
 </sst>
 </file>
@@ -239,9 +241,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -250,27 +270,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -581,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -591,258 +590,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="H17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
-      <c r="H17" s="1" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A19:F26"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A13:F13"/>
     <mergeCell ref="A1:F1"/>
@@ -859,12 +866,6 @@
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="A19:F26"/>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>